<commit_message>
Final touches to data mining
</commit_message>
<xml_diff>
--- a/data/cities.xlsx
+++ b/data/cities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
   <si>
     <t>city</t>
   </si>
@@ -145,7 +145,7 @@
     <t>VOLKSWAGEN 10.6</t>
   </si>
   <si>
-    <t>VOLKSWAGEN 18.3</t>
+    <t>VOLKSWAGEN 18.2</t>
   </si>
   <si>
     <t>VOLKSWAGEN 12.6</t>
@@ -154,16 +154,16 @@
     <t>VOLKSWAGEN 12.4</t>
   </si>
   <si>
-    <t>TOYOTA 10.9</t>
+    <t>TOYOTA 10.8</t>
   </si>
   <si>
     <t>VOLKSWAGEN 9.8</t>
   </si>
   <si>
-    <t>TOYOTA 7.9</t>
-  </si>
-  <si>
-    <t>FORD 8.5</t>
+    <t>TOYOTA 7.8</t>
+  </si>
+  <si>
+    <t>FORD 8.4</t>
   </si>
   <si>
     <t>TOYOTA 10.1</t>
@@ -178,13 +178,13 @@
     <t>VOLKSWAGEN 9.6</t>
   </si>
   <si>
-    <t>VOLKSWAGEN 11.3</t>
+    <t>VOLKSWAGEN 11.2</t>
   </si>
   <si>
     <t>TOYOTA 9.6</t>
   </si>
   <si>
-    <t>AUDI 9.8</t>
+    <t>AUDI 9.7</t>
   </si>
   <si>
     <t>TOYOTA 11.1</t>
@@ -205,9 +205,6 @@
     <t>FORD 7.7</t>
   </si>
   <si>
-    <t>TOYOTA 7.8</t>
-  </si>
-  <si>
     <t>BMW 8.0</t>
   </si>
   <si>
@@ -226,7 +223,10 @@
     <t>KIA 6.8</t>
   </si>
   <si>
-    <t>FORD 9.3</t>
+    <t>TOYOTA 7.5</t>
+  </si>
+  <si>
+    <t>FORD 9.2</t>
   </si>
   <si>
     <t>ŠKODA 6.9</t>
@@ -256,30 +256,33 @@
     <t>PASSAT 2.6</t>
   </si>
   <si>
+    <t>OCTAVIA 2.6</t>
+  </si>
+  <si>
+    <t>AVENSIS 3.2</t>
+  </si>
+  <si>
+    <t>AVENSIS 3.9</t>
+  </si>
+  <si>
+    <t>OCTAVIA 2.8</t>
+  </si>
+  <si>
+    <t>PASSAT VARIANT 4.4</t>
+  </si>
+  <si>
+    <t>AVENSIS 3.1</t>
+  </si>
+  <si>
+    <t>OCTAVIA 3.0</t>
+  </si>
+  <si>
+    <t>CR-V 2.9</t>
+  </si>
+  <si>
     <t>OCTAVIA 2.7</t>
   </si>
   <si>
-    <t>AVENSIS 3.2</t>
-  </si>
-  <si>
-    <t>AVENSIS 3.9</t>
-  </si>
-  <si>
-    <t>OCTAVIA 2.8</t>
-  </si>
-  <si>
-    <t>PASSAT VARIANT 4.4</t>
-  </si>
-  <si>
-    <t>AVENSIS 3.1</t>
-  </si>
-  <si>
-    <t>OCTAVIA 3.0</t>
-  </si>
-  <si>
-    <t>CR-V 2.9</t>
-  </si>
-  <si>
     <t>PASSAT 2.7</t>
   </si>
   <si>
@@ -331,7 +334,7 @@
     <t>AVENSIS 2.9</t>
   </si>
   <si>
-    <t>PASSAT VARIANT 2.6</t>
+    <t>FOCUS 2.6</t>
   </si>
   <si>
     <t>PASSAT 2.5</t>
@@ -768,22 +771,22 @@
         <v>18</v>
       </c>
       <c r="C2">
-        <v>185510</v>
+        <v>186177</v>
       </c>
       <c r="D2">
-        <v>8.970000000000001</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="E2">
-        <v>56.18</v>
+        <v>56.15</v>
       </c>
       <c r="F2">
-        <v>60.65</v>
+        <v>60.43</v>
       </c>
       <c r="G2">
-        <v>39</v>
+        <v>38.86</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -792,13 +795,13 @@
         <v>34</v>
       </c>
       <c r="K2">
-        <v>111.3985445528543</v>
+        <v>111.2536865455991</v>
       </c>
       <c r="L2">
-        <v>162.7126744486268</v>
+        <v>161.9785992086307</v>
       </c>
       <c r="M2">
-        <v>1572.783952347582</v>
+        <v>1572.773930184717</v>
       </c>
       <c r="N2" t="s">
         <v>35</v>
@@ -813,10 +816,10 @@
         <v>75</v>
       </c>
       <c r="R2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="S2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -827,22 +830,22 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>39366</v>
+        <v>39470</v>
       </c>
       <c r="D3">
-        <v>6.57</v>
+        <v>6.56</v>
       </c>
       <c r="E3">
-        <v>46.3</v>
+        <v>46.33</v>
       </c>
       <c r="F3">
-        <v>54.77</v>
+        <v>54.62</v>
       </c>
       <c r="G3">
-        <v>44.74</v>
+        <v>44.63</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="I3" t="s">
         <v>33</v>
@@ -851,13 +854,13 @@
         <v>34</v>
       </c>
       <c r="K3">
-        <v>107.2355281207134</v>
+        <v>107.1201621484672</v>
       </c>
       <c r="L3">
-        <v>164.3450222374273</v>
+        <v>163.7623576736892</v>
       </c>
       <c r="M3">
-        <v>1566.483031042016</v>
+        <v>1566.245604256397</v>
       </c>
       <c r="N3" t="s">
         <v>36</v>
@@ -872,10 +875,10 @@
         <v>76</v>
       </c>
       <c r="R3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -886,22 +889,22 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>22253</v>
+        <v>22295</v>
       </c>
       <c r="D4">
-        <v>7.1</v>
+        <v>7.08</v>
       </c>
       <c r="E4">
         <v>47.49</v>
       </c>
       <c r="F4">
-        <v>54.33</v>
+        <v>54.23</v>
       </c>
       <c r="G4">
-        <v>45.29</v>
+        <v>45.2</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="I4" t="s">
         <v>33</v>
@@ -910,13 +913,13 @@
         <v>34</v>
       </c>
       <c r="K4">
-        <v>106.7504561182762</v>
+        <v>106.6654361964566</v>
       </c>
       <c r="L4">
-        <v>166.580375782881</v>
+        <v>166.1518863302303</v>
       </c>
       <c r="M4">
-        <v>1561.769873724891</v>
+        <v>1561.525140165957</v>
       </c>
       <c r="N4" t="s">
         <v>37</v>
@@ -925,16 +928,16 @@
         <v>49</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="Q4" t="s">
         <v>77</v>
       </c>
       <c r="R4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -945,22 +948,22 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>18760</v>
+        <v>18766</v>
       </c>
       <c r="D5">
         <v>14.77</v>
       </c>
       <c r="E5">
-        <v>40.77</v>
+        <v>40.78</v>
       </c>
       <c r="F5">
-        <v>54.73</v>
+        <v>54.71</v>
       </c>
       <c r="G5">
-        <v>45.14</v>
+        <v>45.13</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -969,13 +972,13 @@
         <v>34</v>
       </c>
       <c r="K5">
-        <v>104.3212846481876</v>
+        <v>104.313615048492</v>
       </c>
       <c r="L5">
-        <v>176.5310729825138</v>
+        <v>176.4441618117666</v>
       </c>
       <c r="M5">
-        <v>1581.439019189766</v>
+        <v>1581.429500159864</v>
       </c>
       <c r="N5" t="s">
         <v>38</v>
@@ -984,16 +987,16 @@
         <v>50</v>
       </c>
       <c r="P5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q5" t="s">
         <v>78</v>
       </c>
       <c r="R5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1004,7 +1007,7 @@
         <v>22</v>
       </c>
       <c r="C6">
-        <v>11682</v>
+        <v>11683</v>
       </c>
       <c r="D6">
         <v>8.25</v>
@@ -1016,10 +1019,10 @@
         <v>41.05</v>
       </c>
       <c r="G6">
-        <v>58.92</v>
+        <v>58.91</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="I6" t="s">
         <v>33</v>
@@ -1028,13 +1031,13 @@
         <v>34</v>
       </c>
       <c r="K6">
-        <v>101.6505992124636</v>
+        <v>101.6444663185825</v>
       </c>
       <c r="L6">
-        <v>168.7968347442032</v>
+        <v>168.7761285574092</v>
       </c>
       <c r="M6">
-        <v>1571.42544084917</v>
+        <v>1571.407943165283</v>
       </c>
       <c r="N6" t="s">
         <v>36</v>
@@ -1043,16 +1046,16 @@
         <v>51</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" t="s">
         <v>79</v>
       </c>
       <c r="R6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1063,22 +1066,22 @@
         <v>23</v>
       </c>
       <c r="C7">
-        <v>7924</v>
+        <v>7953</v>
       </c>
       <c r="D7">
-        <v>7.04</v>
+        <v>7.02</v>
       </c>
       <c r="E7">
-        <v>45.43</v>
+        <v>45.53</v>
       </c>
       <c r="F7">
-        <v>54.35</v>
+        <v>54.16</v>
       </c>
       <c r="G7">
-        <v>45.39</v>
+        <v>45.23</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="I7" t="s">
         <v>33</v>
@@ -1087,13 +1090,13 @@
         <v>34</v>
       </c>
       <c r="K7">
-        <v>104.1413679959616</v>
+        <v>103.9775179177669</v>
       </c>
       <c r="L7">
-        <v>164.2164073550212</v>
+        <v>163.3787159190853</v>
       </c>
       <c r="M7">
-        <v>1544.180590610803</v>
+        <v>1543.728027159562</v>
       </c>
       <c r="N7" t="s">
         <v>39</v>
@@ -1102,16 +1105,16 @@
         <v>52</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q7" t="s">
         <v>80</v>
       </c>
       <c r="R7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="S7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1122,22 +1125,22 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>7087</v>
+        <v>7096</v>
       </c>
       <c r="D8">
-        <v>10.02</v>
+        <v>10.01</v>
       </c>
       <c r="E8">
-        <v>47.33</v>
+        <v>47.29</v>
       </c>
       <c r="F8">
-        <v>53.2</v>
+        <v>53.13</v>
       </c>
       <c r="G8">
-        <v>46.45</v>
+        <v>46.39</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I8" t="s">
         <v>33</v>
@@ -1146,13 +1149,13 @@
         <v>34</v>
       </c>
       <c r="K8">
-        <v>106.1758995343587</v>
+        <v>106.1422773393461</v>
       </c>
       <c r="L8">
-        <v>168.1518602885346</v>
+        <v>167.8650748531363</v>
       </c>
       <c r="M8">
-        <v>1570.496260759136</v>
+        <v>1570.619503945885</v>
       </c>
       <c r="N8" t="s">
         <v>40</v>
@@ -1161,16 +1164,16 @@
         <v>53</v>
       </c>
       <c r="P8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q8" t="s">
         <v>81</v>
       </c>
       <c r="R8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -1181,22 +1184,22 @@
         <v>25</v>
       </c>
       <c r="C9">
-        <v>7084</v>
+        <v>7095</v>
       </c>
       <c r="D9">
-        <v>8.41</v>
+        <v>8.4</v>
       </c>
       <c r="E9">
-        <v>43.32</v>
+        <v>43.38</v>
       </c>
       <c r="F9">
-        <v>53.73</v>
+        <v>53.64</v>
       </c>
       <c r="G9">
-        <v>45.85</v>
+        <v>45.78</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="I9" t="s">
         <v>33</v>
@@ -1205,13 +1208,13 @@
         <v>34</v>
       </c>
       <c r="K9">
-        <v>104.2872106154715</v>
+        <v>104.1938830162086</v>
       </c>
       <c r="L9">
-        <v>164.9237650719564</v>
+        <v>164.5717058024452</v>
       </c>
       <c r="M9">
-        <v>1549.481648785997</v>
+        <v>1549.031994362227</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -1220,16 +1223,16 @@
         <v>54</v>
       </c>
       <c r="P9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="s">
         <v>82</v>
       </c>
       <c r="R9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="S9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1240,22 +1243,22 @@
         <v>26</v>
       </c>
       <c r="C10">
-        <v>6425</v>
+        <v>6429</v>
       </c>
       <c r="D10">
         <v>6.66</v>
       </c>
       <c r="E10">
-        <v>44.98</v>
+        <v>45</v>
       </c>
       <c r="F10">
-        <v>58.24</v>
+        <v>58.21</v>
       </c>
       <c r="G10">
-        <v>40.59</v>
+        <v>40.57</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="I10" t="s">
         <v>33</v>
@@ -1264,13 +1267,13 @@
         <v>34</v>
       </c>
       <c r="K10">
-        <v>102.4559688715953</v>
+        <v>102.4209986000933</v>
       </c>
       <c r="L10">
-        <v>162.6890504704876</v>
+        <v>162.55</v>
       </c>
       <c r="M10">
-        <v>1527.616653696498</v>
+        <v>1527.464613470213</v>
       </c>
       <c r="N10" t="s">
         <v>42</v>
@@ -1279,16 +1282,16 @@
         <v>55</v>
       </c>
       <c r="P10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q10" t="s">
         <v>83</v>
       </c>
       <c r="R10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="S10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -1299,22 +1302,22 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>5588</v>
+        <v>5603</v>
       </c>
       <c r="D11">
-        <v>7.46</v>
+        <v>7.44</v>
       </c>
       <c r="E11">
-        <v>38.71</v>
+        <v>38.85</v>
       </c>
       <c r="F11">
-        <v>46.35</v>
+        <v>46.23</v>
       </c>
       <c r="G11">
-        <v>53.4</v>
+        <v>53.26</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="I11" t="s">
         <v>33</v>
@@ -1323,13 +1326,13 @@
         <v>34</v>
       </c>
       <c r="K11">
-        <v>103.2814781675018</v>
+        <v>103.1067106907014</v>
       </c>
       <c r="L11">
-        <v>165.4732454961011</v>
+        <v>164.8085163363685</v>
       </c>
       <c r="M11">
-        <v>1552.987294201861</v>
+        <v>1552.078529359272</v>
       </c>
       <c r="N11" t="s">
         <v>43</v>
@@ -1338,16 +1341,16 @@
         <v>56</v>
       </c>
       <c r="P11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Q11" t="s">
         <v>84</v>
       </c>
       <c r="R11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -1358,22 +1361,22 @@
         <v>28</v>
       </c>
       <c r="C12">
-        <v>5064</v>
+        <v>5074</v>
       </c>
       <c r="D12">
-        <v>7.9</v>
+        <v>7.88</v>
       </c>
       <c r="E12">
-        <v>39.44</v>
+        <v>39.46</v>
       </c>
       <c r="F12">
-        <v>51.5</v>
+        <v>51.4</v>
       </c>
       <c r="G12">
-        <v>48.28</v>
+        <v>48.19</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
@@ -1382,13 +1385,13 @@
         <v>34</v>
       </c>
       <c r="K12">
-        <v>103.2488941548183</v>
+        <v>103.2046511627907</v>
       </c>
       <c r="L12">
-        <v>165.4926010244735</v>
+        <v>165.0229852440409</v>
       </c>
       <c r="M12">
-        <v>1539.614731437599</v>
+        <v>1539.745368545526</v>
       </c>
       <c r="N12" t="s">
         <v>44</v>
@@ -1403,10 +1406,10 @@
         <v>85</v>
       </c>
       <c r="R12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -1417,22 +1420,22 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>4610</v>
+        <v>4618</v>
       </c>
       <c r="D13">
-        <v>6.81</v>
+        <v>6.8</v>
       </c>
       <c r="E13">
-        <v>49.8</v>
+        <v>49.78</v>
       </c>
       <c r="F13">
-        <v>56.46</v>
+        <v>56.37</v>
       </c>
       <c r="G13">
-        <v>43.34</v>
+        <v>43.27</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="I13" t="s">
         <v>33</v>
@@ -1441,13 +1444,13 @@
         <v>34</v>
       </c>
       <c r="K13">
-        <v>107.1129934924078</v>
+        <v>107.0318103074924</v>
       </c>
       <c r="L13">
-        <v>164.0104786179552</v>
+        <v>163.6397287369313</v>
       </c>
       <c r="M13">
-        <v>1556.386334056399</v>
+        <v>1556.445214378519</v>
       </c>
       <c r="N13" t="s">
         <v>38</v>
@@ -1465,7 +1468,7 @@
         <v>75</v>
       </c>
       <c r="S13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -1476,22 +1479,22 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>4402</v>
+        <v>4403</v>
       </c>
       <c r="D14">
         <v>8.31</v>
       </c>
       <c r="E14">
-        <v>37.66</v>
+        <v>37.68</v>
       </c>
       <c r="F14">
-        <v>48.11</v>
+        <v>48.1</v>
       </c>
       <c r="G14">
-        <v>51.82</v>
+        <v>51.81</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I14" t="s">
         <v>33</v>
@@ -1500,13 +1503,13 @@
         <v>34</v>
       </c>
       <c r="K14">
-        <v>102.64525215811</v>
+        <v>102.6298887122417</v>
       </c>
       <c r="L14">
-        <v>170.5255284552846</v>
+        <v>170.4700910273082</v>
       </c>
       <c r="M14">
-        <v>1567.66855974557</v>
+        <v>1567.581648875767</v>
       </c>
       <c r="N14" t="s">
         <v>36</v>
@@ -1524,7 +1527,7 @@
         <v>75</v>
       </c>
       <c r="S14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -1535,22 +1538,22 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>2243</v>
+        <v>2244</v>
       </c>
       <c r="D15">
-        <v>14.94</v>
+        <v>14.93</v>
       </c>
       <c r="E15">
-        <v>42.76</v>
+        <v>42.74</v>
       </c>
       <c r="F15">
-        <v>50.96</v>
+        <v>50.94</v>
       </c>
       <c r="G15">
-        <v>48.68</v>
+        <v>48.66</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="I15" t="s">
         <v>33</v>
@@ -1559,13 +1562,13 @@
         <v>34</v>
       </c>
       <c r="K15">
-        <v>105.3187695051271</v>
+        <v>105.3025846702317</v>
       </c>
       <c r="L15">
-        <v>175.4271047227926</v>
+        <v>175.3071135430916</v>
       </c>
       <c r="M15">
-        <v>1588.444048149799</v>
+        <v>1588.705436720143</v>
       </c>
       <c r="N15" t="s">
         <v>45</v>
@@ -1580,10 +1583,10 @@
         <v>78</v>
       </c>
       <c r="R15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -1594,22 +1597,22 @@
         <v>32</v>
       </c>
       <c r="C16">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="D16">
-        <v>11.58</v>
+        <v>11.56</v>
       </c>
       <c r="E16">
-        <v>39.95</v>
+        <v>39.98</v>
       </c>
       <c r="F16">
-        <v>56.5</v>
+        <v>56.37</v>
       </c>
       <c r="G16">
-        <v>43.26</v>
+        <v>43.16</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="I16" t="s">
         <v>33</v>
@@ -1618,13 +1621,13 @@
         <v>34</v>
       </c>
       <c r="K16">
-        <v>103.284988179669</v>
+        <v>103.1770047169811</v>
       </c>
       <c r="L16">
-        <v>173.8144876325088</v>
+        <v>173.2024647887324</v>
       </c>
       <c r="M16">
-        <v>1547.496453900709</v>
+        <v>1547.146226415094</v>
       </c>
       <c r="N16" t="s">
         <v>46</v>
@@ -1639,10 +1642,10 @@
         <v>81</v>
       </c>
       <c r="R16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="S16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>